<commit_message>
Actualización general: README, manuales, módulos y reportes
</commit_message>
<xml_diff>
--- a/evaluaciones_tk.xlsx
+++ b/evaluaciones_tk.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,6 +1135,156 @@
         <v>4.2</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>jessica</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" t="n">
+        <v>10</v>
+      </c>
+      <c r="D24" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10</v>
+      </c>
+      <c r="F24" t="n">
+        <v>10</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-07-14 15:32:03</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>marilyn</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" t="n">
+        <v>5</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-07-14 15:34:02</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>4.4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>gypsi</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>10</v>
+      </c>
+      <c r="C26" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10</v>
+      </c>
+      <c r="F26" t="n">
+        <v>10</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-07-14 15:35:49</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>luis</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>7</v>
+      </c>
+      <c r="C27" t="n">
+        <v>9</v>
+      </c>
+      <c r="D27" t="n">
+        <v>5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10</v>
+      </c>
+      <c r="F27" t="n">
+        <v>10</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-07-14 15:37:47</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>8.199999999999999</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>jessica</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10</v>
+      </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10</v>
+      </c>
+      <c r="F28" t="n">
+        <v>10</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-07-14 15:51:55</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>